<commit_message>
Added radio testing stuff
</commit_message>
<xml_diff>
--- a/testing/assembly-checklist.xlsx
+++ b/testing/assembly-checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8a7dff0b441a3a2/Documents/GitHub/flora-hardware/petal-v0_0/testing/internal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8a7dff0b441a3a2/Documents/GitHub/flora-hardware/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="299" documentId="8_{1B2AB5EB-DFEC-9242-9CCC-20ACAB06D546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9A50FF6-52E2-4F94-80ED-DAB40896BF5B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A60C588-DD73-5943-9372-88FD629F3246}"/>
+    <workbookView minimized="1" xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{4A60C588-DD73-5943-9372-88FD629F3246}"/>
   </bookViews>
   <sheets>
     <sheet name="Check List" sheetId="1" r:id="rId1"/>
@@ -838,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96C5BA4-33F7-E147-97CA-18771A61944E}">
   <dimension ref="A1:B48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1766,7 +1766,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D72AFB2-5DB3-4F4D-80B9-1B82C43DFE6F}">
   <dimension ref="A2:G69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>

</xml_diff>